<commit_message>
Loaded latest version of the ESENER data
</commit_message>
<xml_diff>
--- a/endpoints/kettle/admin/categories/resources/origin/Esener_Categories.xlsx
+++ b/endpoints/kettle/admin/categories/resources/origin/Esener_Categories.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2009" sheetId="1" r:id="rId1"/>
     <sheet name="2014" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2009'!$A$1:$K$82</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1639" uniqueCount="579">
   <si>
     <t>ID</t>
   </si>
@@ -1741,6 +1744,18 @@
   </si>
   <si>
     <t>Father_2_ID</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Previous_ID</t>
+  </si>
+  <si>
+    <t>Next_ID</t>
+  </si>
+  <si>
+    <t>Q65_3</t>
   </si>
 </sst>
 </file>
@@ -2124,24 +2139,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="60.7109375" customWidth="1"/>
-    <col min="5" max="5" width="60.85546875" customWidth="1"/>
-    <col min="6" max="6" width="66.85546875" customWidth="1"/>
-    <col min="7" max="7" width="34.140625" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="3.5703125" customWidth="1"/>
+    <col min="6" max="6" width="1" customWidth="1"/>
+    <col min="7" max="7" width="85.85546875" customWidth="1"/>
+    <col min="8" max="8" width="2.28515625" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2166,8 +2183,17 @@
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -2177,8 +2203,11 @@
       <c r="F2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
@@ -2191,8 +2220,11 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>173</v>
       </c>
@@ -2211,8 +2243,17 @@
       <c r="H4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>174</v>
       </c>
@@ -2231,8 +2272,17 @@
       <c r="H5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>9</v>
+      </c>
+      <c r="J5" t="s">
+        <v>173</v>
+      </c>
+      <c r="K5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>175</v>
       </c>
@@ -2251,8 +2301,17 @@
       <c r="H6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>174</v>
+      </c>
+      <c r="K6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>176</v>
       </c>
@@ -2271,8 +2330,17 @@
       <c r="H7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>11</v>
+      </c>
+      <c r="J7" t="s">
+        <v>175</v>
+      </c>
+      <c r="K7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>177</v>
       </c>
@@ -2291,8 +2359,17 @@
       <c r="H8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>12</v>
+      </c>
+      <c r="J8" t="s">
+        <v>176</v>
+      </c>
+      <c r="K8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>178</v>
       </c>
@@ -2311,8 +2388,17 @@
       <c r="H9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>13</v>
+      </c>
+      <c r="J9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>179</v>
       </c>
@@ -2331,8 +2417,17 @@
       <c r="H10" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>14</v>
+      </c>
+      <c r="J10" t="s">
+        <v>178</v>
+      </c>
+      <c r="K10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>181</v>
       </c>
@@ -2351,8 +2446,17 @@
       <c r="H11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>15</v>
+      </c>
+      <c r="J11" t="s">
+        <v>179</v>
+      </c>
+      <c r="K11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>2</v>
       </c>
@@ -2365,8 +2469,11 @@
       <c r="F12" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>180</v>
       </c>
@@ -2385,8 +2492,17 @@
       <c r="H13" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>25</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="K13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2</v>
       </c>
@@ -2399,8 +2515,11 @@
       <c r="F14" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -2425,8 +2544,14 @@
       <c r="H15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="K15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2451,8 +2576,17 @@
       <c r="H16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -2477,8 +2611,17 @@
       <c r="H17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="J17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2503,8 +2646,17 @@
       <c r="H18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>6</v>
+      </c>
+      <c r="J18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -2529,8 +2681,17 @@
       <c r="H19" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>7</v>
+      </c>
+      <c r="J19" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>182</v>
       </c>
@@ -2555,8 +2716,17 @@
       <c r="H20" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>17</v>
+      </c>
+      <c r="J20" t="s">
+        <v>181</v>
+      </c>
+      <c r="K20" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>183</v>
       </c>
@@ -2581,8 +2751,17 @@
       <c r="H21" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>18</v>
+      </c>
+      <c r="J21" t="s">
+        <v>182</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>184</v>
       </c>
@@ -2607,8 +2786,17 @@
       <c r="H22" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>19</v>
+      </c>
+      <c r="J22" t="s">
+        <v>183</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>185</v>
       </c>
@@ -2633,8 +2821,17 @@
       <c r="H23" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>20</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>186</v>
       </c>
@@ -2659,8 +2856,17 @@
       <c r="H24" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>21</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>187</v>
       </c>
@@ -2685,8 +2891,17 @@
       <c r="H25" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>22</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="K25" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>188</v>
       </c>
@@ -2711,8 +2926,17 @@
       <c r="H26" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>23</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>189</v>
       </c>
@@ -2737,8 +2961,17 @@
       <c r="H27" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>24</v>
+      </c>
+      <c r="J27" t="s">
+        <v>189</v>
+      </c>
+      <c r="K27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>190</v>
       </c>
@@ -2763,8 +2996,17 @@
       <c r="H28" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>27</v>
+      </c>
+      <c r="J28" t="s">
+        <v>180</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>191</v>
       </c>
@@ -2789,8 +3031,17 @@
       <c r="H29" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>28</v>
+      </c>
+      <c r="J29" t="s">
+        <v>190</v>
+      </c>
+      <c r="K29" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>192</v>
       </c>
@@ -2815,8 +3066,17 @@
       <c r="H30" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>29</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>193</v>
       </c>
@@ -2841,8 +3101,17 @@
       <c r="H31" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>30</v>
+      </c>
+      <c r="J31" t="s">
+        <v>192</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>194</v>
       </c>
@@ -2867,8 +3136,17 @@
       <c r="H32" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>31</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>195</v>
       </c>
@@ -2893,8 +3171,17 @@
       <c r="H33" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>32</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>196</v>
       </c>
@@ -2919,8 +3206,17 @@
       <c r="H34" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>33</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>1</v>
       </c>
@@ -2930,8 +3226,11 @@
       <c r="F35" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>2</v>
       </c>
@@ -2944,8 +3243,11 @@
       <c r="F36" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>207</v>
       </c>
@@ -2964,8 +3266,17 @@
       <c r="H37" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>46</v>
+      </c>
+      <c r="J37" t="s">
+        <v>206</v>
+      </c>
+      <c r="K37" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>209</v>
       </c>
@@ -2984,8 +3295,17 @@
       <c r="H38" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>47</v>
+      </c>
+      <c r="J38" t="s">
+        <v>207</v>
+      </c>
+      <c r="K38" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>210</v>
       </c>
@@ -3004,8 +3324,17 @@
       <c r="H39" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>48</v>
+      </c>
+      <c r="J39" t="s">
+        <v>209</v>
+      </c>
+      <c r="K39" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>2</v>
       </c>
@@ -3018,8 +3347,11 @@
       <c r="F40" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>217</v>
       </c>
@@ -3038,8 +3370,17 @@
       <c r="H41" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>56</v>
+      </c>
+      <c r="J41" t="s">
+        <v>216</v>
+      </c>
+      <c r="K41" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>218</v>
       </c>
@@ -3058,8 +3399,17 @@
       <c r="H42" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>57</v>
+      </c>
+      <c r="J42" t="s">
+        <v>217</v>
+      </c>
+      <c r="K42" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>219</v>
       </c>
@@ -3078,8 +3428,17 @@
       <c r="H43" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>58</v>
+      </c>
+      <c r="J43" t="s">
+        <v>218</v>
+      </c>
+      <c r="K43" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>197</v>
       </c>
@@ -3104,8 +3463,17 @@
       <c r="H44" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>36</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="K44" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>198</v>
       </c>
@@ -3130,8 +3498,17 @@
       <c r="H45" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>37</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="K45" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>199</v>
       </c>
@@ -3156,8 +3533,17 @@
       <c r="H46" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>38</v>
+      </c>
+      <c r="J46" t="s">
+        <v>198</v>
+      </c>
+      <c r="K46" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>200</v>
       </c>
@@ -3182,8 +3568,17 @@
       <c r="H47" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>39</v>
+      </c>
+      <c r="J47" t="s">
+        <v>199</v>
+      </c>
+      <c r="K47" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>201</v>
       </c>
@@ -3208,8 +3603,17 @@
       <c r="H48" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>40</v>
+      </c>
+      <c r="J48" t="s">
+        <v>200</v>
+      </c>
+      <c r="K48" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>202</v>
       </c>
@@ -3234,8 +3638,17 @@
       <c r="H49" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <v>41</v>
+      </c>
+      <c r="J49" t="s">
+        <v>201</v>
+      </c>
+      <c r="K49" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>203</v>
       </c>
@@ -3260,8 +3673,17 @@
       <c r="H50" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <v>42</v>
+      </c>
+      <c r="J50" t="s">
+        <v>202</v>
+      </c>
+      <c r="K50" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>204</v>
       </c>
@@ -3286,8 +3708,17 @@
       <c r="H51" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <v>43</v>
+      </c>
+      <c r="J51" t="s">
+        <v>203</v>
+      </c>
+      <c r="K51" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>205</v>
       </c>
@@ -3312,8 +3743,17 @@
       <c r="H52" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52">
+        <v>44</v>
+      </c>
+      <c r="J52" t="s">
+        <v>204</v>
+      </c>
+      <c r="K52" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>206</v>
       </c>
@@ -3338,8 +3778,17 @@
       <c r="H53" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <v>45</v>
+      </c>
+      <c r="J53" t="s">
+        <v>205</v>
+      </c>
+      <c r="K53" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>211</v>
       </c>
@@ -3364,8 +3813,17 @@
       <c r="H54" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54">
+        <v>50</v>
+      </c>
+      <c r="J54" t="s">
+        <v>210</v>
+      </c>
+      <c r="K54" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>212</v>
       </c>
@@ -3390,8 +3848,17 @@
       <c r="H55" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55">
+        <v>51</v>
+      </c>
+      <c r="J55" t="s">
+        <v>211</v>
+      </c>
+      <c r="K55" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>213</v>
       </c>
@@ -3416,8 +3883,17 @@
       <c r="H56" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56">
+        <v>52</v>
+      </c>
+      <c r="J56" t="s">
+        <v>212</v>
+      </c>
+      <c r="K56" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>214</v>
       </c>
@@ -3442,8 +3918,17 @@
       <c r="H57" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57">
+        <v>53</v>
+      </c>
+      <c r="J57" t="s">
+        <v>213</v>
+      </c>
+      <c r="K57" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>215</v>
       </c>
@@ -3468,8 +3953,17 @@
       <c r="H58" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58">
+        <v>54</v>
+      </c>
+      <c r="J58" t="s">
+        <v>214</v>
+      </c>
+      <c r="K58" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>216</v>
       </c>
@@ -3494,8 +3988,17 @@
       <c r="H59" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59">
+        <v>55</v>
+      </c>
+      <c r="J59" t="s">
+        <v>215</v>
+      </c>
+      <c r="K59" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>1</v>
       </c>
@@ -3505,8 +4008,11 @@
       <c r="F60" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>2</v>
       </c>
@@ -3519,8 +4025,11 @@
       <c r="F61" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>2</v>
       </c>
@@ -3533,8 +4042,11 @@
       <c r="F62" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>235</v>
       </c>
@@ -3553,8 +4065,17 @@
       <c r="H63" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63">
+        <v>72</v>
+      </c>
+      <c r="J63" t="s">
+        <v>231</v>
+      </c>
+      <c r="K63" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>236</v>
       </c>
@@ -3573,8 +4094,17 @@
       <c r="H64" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64">
+        <v>73</v>
+      </c>
+      <c r="J64" t="s">
+        <v>235</v>
+      </c>
+      <c r="K64" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>237</v>
       </c>
@@ -3593,8 +4123,17 @@
       <c r="H65" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65">
+        <v>74</v>
+      </c>
+      <c r="J65" t="s">
+        <v>236</v>
+      </c>
+      <c r="K65" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>220</v>
       </c>
@@ -3619,8 +4158,17 @@
       <c r="H66" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66">
+        <v>59</v>
+      </c>
+      <c r="J66" t="s">
+        <v>219</v>
+      </c>
+      <c r="K66" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>221</v>
       </c>
@@ -3645,8 +4193,17 @@
       <c r="H67" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67">
+        <v>60</v>
+      </c>
+      <c r="J67" t="s">
+        <v>220</v>
+      </c>
+      <c r="K67" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>222</v>
       </c>
@@ -3671,8 +4228,17 @@
       <c r="H68" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I68">
+        <v>61</v>
+      </c>
+      <c r="J68" t="s">
+        <v>221</v>
+      </c>
+      <c r="K68" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>223</v>
       </c>
@@ -3697,8 +4263,17 @@
       <c r="H69" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69">
+        <v>62</v>
+      </c>
+      <c r="J69" t="s">
+        <v>222</v>
+      </c>
+      <c r="K69" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>224</v>
       </c>
@@ -3723,8 +4298,17 @@
       <c r="H70" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70">
+        <v>63</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="K70" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>225</v>
       </c>
@@ -3749,8 +4333,17 @@
       <c r="H71" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71">
+        <v>64</v>
+      </c>
+      <c r="J71" t="s">
+        <v>224</v>
+      </c>
+      <c r="K71" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>226</v>
       </c>
@@ -3775,8 +4368,17 @@
       <c r="H72" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72">
+        <v>66</v>
+      </c>
+      <c r="J72" t="s">
+        <v>225</v>
+      </c>
+      <c r="K72" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>227</v>
       </c>
@@ -3801,8 +4403,17 @@
       <c r="H73" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73">
+        <v>67</v>
+      </c>
+      <c r="J73" t="s">
+        <v>226</v>
+      </c>
+      <c r="K73" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>228</v>
       </c>
@@ -3827,8 +4438,17 @@
       <c r="H74" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74">
+        <v>68</v>
+      </c>
+      <c r="J74" t="s">
+        <v>227</v>
+      </c>
+      <c r="K74" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>229</v>
       </c>
@@ -3853,8 +4473,17 @@
       <c r="H75" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75">
+        <v>69</v>
+      </c>
+      <c r="J75" t="s">
+        <v>228</v>
+      </c>
+      <c r="K75" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>230</v>
       </c>
@@ -3879,8 +4508,17 @@
       <c r="H76" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76">
+        <v>70</v>
+      </c>
+      <c r="J76" t="s">
+        <v>229</v>
+      </c>
+      <c r="K76" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>231</v>
       </c>
@@ -3905,8 +4543,17 @@
       <c r="H77" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77">
+        <v>71</v>
+      </c>
+      <c r="J77" t="s">
+        <v>230</v>
+      </c>
+      <c r="K77" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>1</v>
       </c>
@@ -3916,8 +4563,11 @@
       <c r="F78" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>208</v>
       </c>
@@ -3936,8 +4586,17 @@
       <c r="H79" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79">
+        <v>76</v>
+      </c>
+      <c r="J79" t="s">
+        <v>237</v>
+      </c>
+      <c r="K79" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>232</v>
       </c>
@@ -3956,8 +4615,17 @@
       <c r="H80" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80">
+        <v>77</v>
+      </c>
+      <c r="J80" t="s">
+        <v>208</v>
+      </c>
+      <c r="K80" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>233</v>
       </c>
@@ -3976,8 +4644,17 @@
       <c r="H81" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81">
+        <v>78</v>
+      </c>
+      <c r="J81" t="s">
+        <v>232</v>
+      </c>
+      <c r="K81" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>234</v>
       </c>
@@ -3996,8 +4673,15 @@
       <c r="H82" t="s">
         <v>172</v>
       </c>
+      <c r="I82">
+        <v>79</v>
+      </c>
+      <c r="J82" t="s">
+        <v>233</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K82"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4005,24 +4689,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H129"/>
+  <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" customWidth="1"/>
-    <col min="4" max="4" width="55.28515625" customWidth="1"/>
-    <col min="5" max="5" width="50.7109375" customWidth="1"/>
-    <col min="6" max="6" width="162.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="1" max="2" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
+    <col min="7" max="7" width="39.85546875" customWidth="1"/>
+    <col min="8" max="8" width="33.140625" customWidth="1"/>
+    <col min="9" max="9" width="39.7109375" customWidth="1"/>
+    <col min="10" max="10" width="115.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4047,8 +4733,17 @@
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -4058,8 +4753,11 @@
       <c r="F2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
@@ -4072,8 +4770,11 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>465</v>
       </c>
@@ -4098,8 +4799,14 @@
       <c r="H4" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>466</v>
       </c>
@@ -4124,8 +4831,17 @@
       <c r="H5" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>465</v>
+      </c>
+      <c r="K5" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>467</v>
       </c>
@@ -4150,8 +4866,17 @@
       <c r="H6" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6" t="s">
+        <v>466</v>
+      </c>
+      <c r="K6" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>468</v>
       </c>
@@ -4176,8 +4901,17 @@
       <c r="H7" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7" t="s">
+        <v>467</v>
+      </c>
+      <c r="K7" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>469</v>
       </c>
@@ -4202,8 +4936,17 @@
       <c r="H8" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8" t="s">
+        <v>468</v>
+      </c>
+      <c r="K8" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>464</v>
       </c>
@@ -4225,8 +4968,17 @@
       <c r="H9" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>469</v>
+      </c>
+      <c r="K9" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>470</v>
       </c>
@@ -4248,8 +5000,17 @@
       <c r="H10" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10" t="s">
+        <v>464</v>
+      </c>
+      <c r="K10" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2</v>
       </c>
@@ -4262,8 +5023,11 @@
       <c r="F11" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>471</v>
       </c>
@@ -4288,8 +5052,17 @@
       <c r="H12" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>11</v>
+      </c>
+      <c r="J12" t="s">
+        <v>470</v>
+      </c>
+      <c r="K12" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>472</v>
       </c>
@@ -4314,8 +5087,17 @@
       <c r="H13" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>12</v>
+      </c>
+      <c r="J13" t="s">
+        <v>471</v>
+      </c>
+      <c r="K13" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>473</v>
       </c>
@@ -4340,8 +5122,17 @@
       <c r="H14" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>13</v>
+      </c>
+      <c r="J14" t="s">
+        <v>472</v>
+      </c>
+      <c r="K14" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>474</v>
       </c>
@@ -4366,8 +5157,17 @@
       <c r="H15" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>14</v>
+      </c>
+      <c r="J15" t="s">
+        <v>473</v>
+      </c>
+      <c r="K15" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>475</v>
       </c>
@@ -4389,8 +5189,17 @@
       <c r="H16" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>15</v>
+      </c>
+      <c r="J16" t="s">
+        <v>474</v>
+      </c>
+      <c r="K16" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>476</v>
       </c>
@@ -4406,11 +5215,23 @@
       <c r="F17" t="s">
         <v>29</v>
       </c>
+      <c r="G17" t="s">
+        <v>29</v>
+      </c>
       <c r="H17" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>16</v>
+      </c>
+      <c r="J17" t="s">
+        <v>475</v>
+      </c>
+      <c r="K17" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>2</v>
       </c>
@@ -4423,8 +5244,11 @@
       <c r="F18" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>477</v>
       </c>
@@ -4449,8 +5273,17 @@
       <c r="H19" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>18</v>
+      </c>
+      <c r="J19" t="s">
+        <v>476</v>
+      </c>
+      <c r="K19" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>478</v>
       </c>
@@ -4475,8 +5308,17 @@
       <c r="H20" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>19</v>
+      </c>
+      <c r="J20" t="s">
+        <v>477</v>
+      </c>
+      <c r="K20" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>479</v>
       </c>
@@ -4501,8 +5343,17 @@
       <c r="H21" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>20</v>
+      </c>
+      <c r="J21" t="s">
+        <v>478</v>
+      </c>
+      <c r="K21" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>480</v>
       </c>
@@ -4527,8 +5378,17 @@
       <c r="H22" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>21</v>
+      </c>
+      <c r="J22" t="s">
+        <v>479</v>
+      </c>
+      <c r="K22" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>481</v>
       </c>
@@ -4553,8 +5413,17 @@
       <c r="H23" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>22</v>
+      </c>
+      <c r="J23" t="s">
+        <v>480</v>
+      </c>
+      <c r="K23" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>482</v>
       </c>
@@ -4576,8 +5445,17 @@
       <c r="G24" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>23</v>
+      </c>
+      <c r="J24" t="s">
+        <v>481</v>
+      </c>
+      <c r="K24" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>483</v>
       </c>
@@ -4602,8 +5480,17 @@
       <c r="H25" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>24</v>
+      </c>
+      <c r="J25" t="s">
+        <v>482</v>
+      </c>
+      <c r="K25" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>484</v>
       </c>
@@ -4628,8 +5515,17 @@
       <c r="H26" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>25</v>
+      </c>
+      <c r="J26" t="s">
+        <v>483</v>
+      </c>
+      <c r="K26" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>485</v>
       </c>
@@ -4654,8 +5550,17 @@
       <c r="H27" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>26</v>
+      </c>
+      <c r="J27" t="s">
+        <v>484</v>
+      </c>
+      <c r="K27" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>2</v>
       </c>
@@ -4668,8 +5573,11 @@
       <c r="F28" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>486</v>
       </c>
@@ -4694,8 +5602,17 @@
       <c r="H29" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>28</v>
+      </c>
+      <c r="J29" t="s">
+        <v>485</v>
+      </c>
+      <c r="K29" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>487</v>
       </c>
@@ -4720,8 +5637,17 @@
       <c r="H30" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>29</v>
+      </c>
+      <c r="J30" t="s">
+        <v>486</v>
+      </c>
+      <c r="K30" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>488</v>
       </c>
@@ -4746,8 +5672,17 @@
       <c r="H31" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>30</v>
+      </c>
+      <c r="J31" t="s">
+        <v>487</v>
+      </c>
+      <c r="K31" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>489</v>
       </c>
@@ -4772,8 +5707,17 @@
       <c r="H32" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>31</v>
+      </c>
+      <c r="J32" t="s">
+        <v>488</v>
+      </c>
+      <c r="K32" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>490</v>
       </c>
@@ -4798,8 +5742,17 @@
       <c r="H33" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>32</v>
+      </c>
+      <c r="J33" t="s">
+        <v>489</v>
+      </c>
+      <c r="K33" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>491</v>
       </c>
@@ -4824,8 +5777,17 @@
       <c r="H34" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>33</v>
+      </c>
+      <c r="J34" t="s">
+        <v>490</v>
+      </c>
+      <c r="K34" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>492</v>
       </c>
@@ -4850,8 +5812,17 @@
       <c r="H35" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>34</v>
+      </c>
+      <c r="J35" t="s">
+        <v>491</v>
+      </c>
+      <c r="K35" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>493</v>
       </c>
@@ -4876,8 +5847,17 @@
       <c r="H36" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>35</v>
+      </c>
+      <c r="J36" t="s">
+        <v>492</v>
+      </c>
+      <c r="K36" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>494</v>
       </c>
@@ -4902,8 +5882,17 @@
       <c r="H37" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>36</v>
+      </c>
+      <c r="J37" t="s">
+        <v>493</v>
+      </c>
+      <c r="K37" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>495</v>
       </c>
@@ -4925,8 +5914,17 @@
       <c r="H38" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>37</v>
+      </c>
+      <c r="J38" t="s">
+        <v>494</v>
+      </c>
+      <c r="K38" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>496</v>
       </c>
@@ -4948,8 +5946,17 @@
       <c r="H39" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>38</v>
+      </c>
+      <c r="J39" t="s">
+        <v>495</v>
+      </c>
+      <c r="K39" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>2</v>
       </c>
@@ -4962,8 +5969,11 @@
       <c r="F40" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>497</v>
       </c>
@@ -4988,8 +5998,17 @@
       <c r="H41" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>40</v>
+      </c>
+      <c r="J41" t="s">
+        <v>496</v>
+      </c>
+      <c r="K41" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>498</v>
       </c>
@@ -5014,8 +6033,17 @@
       <c r="H42" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>41</v>
+      </c>
+      <c r="J42" t="s">
+        <v>497</v>
+      </c>
+      <c r="K42" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>499</v>
       </c>
@@ -5040,8 +6068,17 @@
       <c r="H43" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>42</v>
+      </c>
+      <c r="J43" t="s">
+        <v>498</v>
+      </c>
+      <c r="K43" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>500</v>
       </c>
@@ -5066,8 +6103,17 @@
       <c r="H44" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>43</v>
+      </c>
+      <c r="J44" t="s">
+        <v>499</v>
+      </c>
+      <c r="K44" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>501</v>
       </c>
@@ -5092,8 +6138,17 @@
       <c r="H45" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>44</v>
+      </c>
+      <c r="J45" t="s">
+        <v>500</v>
+      </c>
+      <c r="K45" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>502</v>
       </c>
@@ -5118,8 +6173,17 @@
       <c r="H46" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>45</v>
+      </c>
+      <c r="J46" t="s">
+        <v>501</v>
+      </c>
+      <c r="K46" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>503</v>
       </c>
@@ -5141,8 +6205,17 @@
       <c r="H47" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>46</v>
+      </c>
+      <c r="J47" t="s">
+        <v>502</v>
+      </c>
+      <c r="K47" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>504</v>
       </c>
@@ -5164,8 +6237,17 @@
       <c r="H48" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>47</v>
+      </c>
+      <c r="J48" t="s">
+        <v>503</v>
+      </c>
+      <c r="K48" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>2</v>
       </c>
@@ -5178,8 +6260,11 @@
       <c r="F49" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>505</v>
       </c>
@@ -5204,8 +6289,17 @@
       <c r="H50" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <v>49</v>
+      </c>
+      <c r="J50" t="s">
+        <v>504</v>
+      </c>
+      <c r="K50" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>506</v>
       </c>
@@ -5230,8 +6324,17 @@
       <c r="H51" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <v>50</v>
+      </c>
+      <c r="J51" t="s">
+        <v>505</v>
+      </c>
+      <c r="K51" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>507</v>
       </c>
@@ -5256,8 +6359,17 @@
       <c r="H52" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52">
+        <v>51</v>
+      </c>
+      <c r="J52" t="s">
+        <v>506</v>
+      </c>
+      <c r="K52" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>508</v>
       </c>
@@ -5282,8 +6394,17 @@
       <c r="H53" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <v>52</v>
+      </c>
+      <c r="J53" t="s">
+        <v>507</v>
+      </c>
+      <c r="K53" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>509</v>
       </c>
@@ -5308,8 +6429,17 @@
       <c r="H54" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54">
+        <v>53</v>
+      </c>
+      <c r="J54" t="s">
+        <v>508</v>
+      </c>
+      <c r="K54" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>510</v>
       </c>
@@ -5331,8 +6461,17 @@
       <c r="H55" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55">
+        <v>54</v>
+      </c>
+      <c r="J55" t="s">
+        <v>509</v>
+      </c>
+      <c r="K55" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>2</v>
       </c>
@@ -5345,8 +6484,11 @@
       <c r="F56" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>511</v>
       </c>
@@ -5371,8 +6513,17 @@
       <c r="H57" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57">
+        <v>56</v>
+      </c>
+      <c r="J57" t="s">
+        <v>510</v>
+      </c>
+      <c r="K57" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>512</v>
       </c>
@@ -5397,8 +6548,17 @@
       <c r="H58" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58">
+        <v>57</v>
+      </c>
+      <c r="J58" t="s">
+        <v>511</v>
+      </c>
+      <c r="K58" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>513</v>
       </c>
@@ -5423,8 +6583,17 @@
       <c r="H59" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59">
+        <v>58</v>
+      </c>
+      <c r="J59" t="s">
+        <v>512</v>
+      </c>
+      <c r="K59" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>514</v>
       </c>
@@ -5449,8 +6618,17 @@
       <c r="H60" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60">
+        <v>59</v>
+      </c>
+      <c r="J60" t="s">
+        <v>513</v>
+      </c>
+      <c r="K60" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>2</v>
       </c>
@@ -5463,8 +6641,11 @@
       <c r="F61" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>515</v>
       </c>
@@ -5489,8 +6670,17 @@
       <c r="H62" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62">
+        <v>61</v>
+      </c>
+      <c r="J62" t="s">
+        <v>514</v>
+      </c>
+      <c r="K62" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>516</v>
       </c>
@@ -5515,8 +6705,17 @@
       <c r="H63" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63">
+        <v>62</v>
+      </c>
+      <c r="J63" t="s">
+        <v>515</v>
+      </c>
+      <c r="K63" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>517</v>
       </c>
@@ -5541,8 +6740,17 @@
       <c r="H64" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64">
+        <v>63</v>
+      </c>
+      <c r="J64" t="s">
+        <v>516</v>
+      </c>
+      <c r="K64" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>518</v>
       </c>
@@ -5567,8 +6775,17 @@
       <c r="H65" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65">
+        <v>64</v>
+      </c>
+      <c r="J65" t="s">
+        <v>517</v>
+      </c>
+      <c r="K65" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>2</v>
       </c>
@@ -5581,8 +6798,11 @@
       <c r="F66" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>519</v>
       </c>
@@ -5607,8 +6827,17 @@
       <c r="H67" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67">
+        <v>66</v>
+      </c>
+      <c r="J67" t="s">
+        <v>518</v>
+      </c>
+      <c r="K67" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>520</v>
       </c>
@@ -5633,8 +6862,17 @@
       <c r="H68" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68">
+        <v>67</v>
+      </c>
+      <c r="J68" t="s">
+        <v>519</v>
+      </c>
+      <c r="K68" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>521</v>
       </c>
@@ -5659,8 +6897,17 @@
       <c r="H69" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69">
+        <v>68</v>
+      </c>
+      <c r="J69" t="s">
+        <v>520</v>
+      </c>
+      <c r="K69" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>522</v>
       </c>
@@ -5685,8 +6932,17 @@
       <c r="H70" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70">
+        <v>69</v>
+      </c>
+      <c r="J70" t="s">
+        <v>521</v>
+      </c>
+      <c r="K70" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>523</v>
       </c>
@@ -5711,8 +6967,17 @@
       <c r="H71" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71">
+        <v>70</v>
+      </c>
+      <c r="J71" t="s">
+        <v>522</v>
+      </c>
+      <c r="K71" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>1</v>
       </c>
@@ -5722,8 +6987,11 @@
       <c r="F72" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>2</v>
       </c>
@@ -5736,8 +7004,11 @@
       <c r="F73" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>524</v>
       </c>
@@ -5762,8 +7033,17 @@
       <c r="H74" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74">
+        <v>73</v>
+      </c>
+      <c r="J74" t="s">
+        <v>523</v>
+      </c>
+      <c r="K74" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>525</v>
       </c>
@@ -5788,8 +7068,17 @@
       <c r="H75" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75">
+        <v>74</v>
+      </c>
+      <c r="J75" t="s">
+        <v>524</v>
+      </c>
+      <c r="K75" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>526</v>
       </c>
@@ -5814,8 +7103,17 @@
       <c r="H76" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76">
+        <v>75</v>
+      </c>
+      <c r="J76" t="s">
+        <v>525</v>
+      </c>
+      <c r="K76" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>527</v>
       </c>
@@ -5840,8 +7138,17 @@
       <c r="H77" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77">
+        <v>76</v>
+      </c>
+      <c r="J77" t="s">
+        <v>526</v>
+      </c>
+      <c r="K77" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>528</v>
       </c>
@@ -5866,8 +7173,17 @@
       <c r="H78" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78">
+        <v>77</v>
+      </c>
+      <c r="J78" t="s">
+        <v>527</v>
+      </c>
+      <c r="K78" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>529</v>
       </c>
@@ -5892,8 +7208,17 @@
       <c r="H79" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79">
+        <v>78</v>
+      </c>
+      <c r="J79" t="s">
+        <v>528</v>
+      </c>
+      <c r="K79" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>530</v>
       </c>
@@ -5918,8 +7243,17 @@
       <c r="H80" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80">
+        <v>79</v>
+      </c>
+      <c r="J80" t="s">
+        <v>529</v>
+      </c>
+      <c r="K80" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>2</v>
       </c>
@@ -5932,8 +7266,11 @@
       <c r="F81" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>531</v>
       </c>
@@ -5958,8 +7295,17 @@
       <c r="H82" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82">
+        <v>81</v>
+      </c>
+      <c r="J82" t="s">
+        <v>530</v>
+      </c>
+      <c r="K82" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>532</v>
       </c>
@@ -5984,8 +7330,17 @@
       <c r="H83" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83">
+        <v>82</v>
+      </c>
+      <c r="J83" t="s">
+        <v>531</v>
+      </c>
+      <c r="K83" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>533</v>
       </c>
@@ -6010,8 +7365,17 @@
       <c r="H84" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84">
+        <v>83</v>
+      </c>
+      <c r="J84" t="s">
+        <v>532</v>
+      </c>
+      <c r="K84" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>534</v>
       </c>
@@ -6036,8 +7400,17 @@
       <c r="H85" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85">
+        <v>84</v>
+      </c>
+      <c r="J85" t="s">
+        <v>533</v>
+      </c>
+      <c r="K85" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>535</v>
       </c>
@@ -6062,8 +7435,17 @@
       <c r="H86" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86">
+        <v>85</v>
+      </c>
+      <c r="J86" t="s">
+        <v>534</v>
+      </c>
+      <c r="K86" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>536</v>
       </c>
@@ -6088,8 +7470,17 @@
       <c r="H87" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87">
+        <v>86</v>
+      </c>
+      <c r="J87" t="s">
+        <v>535</v>
+      </c>
+      <c r="K87" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>537</v>
       </c>
@@ -6111,8 +7502,17 @@
       <c r="H88" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88">
+        <v>87</v>
+      </c>
+      <c r="J88" t="s">
+        <v>536</v>
+      </c>
+      <c r="K88" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>538</v>
       </c>
@@ -6134,8 +7534,17 @@
       <c r="H89" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89">
+        <v>88</v>
+      </c>
+      <c r="J89" t="s">
+        <v>537</v>
+      </c>
+      <c r="K89" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>539</v>
       </c>
@@ -6157,8 +7566,17 @@
       <c r="H90" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90">
+        <v>89</v>
+      </c>
+      <c r="J90" t="s">
+        <v>538</v>
+      </c>
+      <c r="K90" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>2</v>
       </c>
@@ -6171,8 +7589,11 @@
       <c r="F91" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>540</v>
       </c>
@@ -6197,8 +7618,17 @@
       <c r="H92" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92">
+        <v>91</v>
+      </c>
+      <c r="J92" t="s">
+        <v>539</v>
+      </c>
+      <c r="K92" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>541</v>
       </c>
@@ -6223,8 +7653,17 @@
       <c r="H93" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93">
+        <v>92</v>
+      </c>
+      <c r="J93" t="s">
+        <v>540</v>
+      </c>
+      <c r="K93" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>542</v>
       </c>
@@ -6249,8 +7688,17 @@
       <c r="H94" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94">
+        <v>93</v>
+      </c>
+      <c r="J94" t="s">
+        <v>541</v>
+      </c>
+      <c r="K94" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>543</v>
       </c>
@@ -6275,8 +7723,17 @@
       <c r="H95" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95">
+        <v>94</v>
+      </c>
+      <c r="J95" t="s">
+        <v>542</v>
+      </c>
+      <c r="K95" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>544</v>
       </c>
@@ -6298,8 +7755,17 @@
       <c r="H96" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96">
+        <v>95</v>
+      </c>
+      <c r="J96" t="s">
+        <v>543</v>
+      </c>
+      <c r="K96" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>1</v>
       </c>
@@ -6309,8 +7775,11 @@
       <c r="F97" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>2</v>
       </c>
@@ -6323,8 +7792,11 @@
       <c r="F98" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>545</v>
       </c>
@@ -6349,8 +7821,17 @@
       <c r="H99" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99">
+        <v>98</v>
+      </c>
+      <c r="J99" t="s">
+        <v>544</v>
+      </c>
+      <c r="K99" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>546</v>
       </c>
@@ -6375,8 +7856,17 @@
       <c r="H100" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I100">
+        <v>99</v>
+      </c>
+      <c r="J100" t="s">
+        <v>545</v>
+      </c>
+      <c r="K100" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>547</v>
       </c>
@@ -6401,8 +7891,17 @@
       <c r="H101" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101">
+        <v>100</v>
+      </c>
+      <c r="J101" t="s">
+        <v>546</v>
+      </c>
+      <c r="K101" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>548</v>
       </c>
@@ -6427,8 +7926,17 @@
       <c r="H102" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I102">
+        <v>101</v>
+      </c>
+      <c r="J102" t="s">
+        <v>547</v>
+      </c>
+      <c r="K102" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>549</v>
       </c>
@@ -6453,8 +7961,17 @@
       <c r="H103" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I103">
+        <v>102</v>
+      </c>
+      <c r="J103" t="s">
+        <v>548</v>
+      </c>
+      <c r="K103" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B104">
         <v>2</v>
       </c>
@@ -6467,8 +7984,11 @@
       <c r="F104" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I104">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>550</v>
       </c>
@@ -6493,8 +8013,17 @@
       <c r="H105" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I105">
+        <v>104</v>
+      </c>
+      <c r="J105" t="s">
+        <v>549</v>
+      </c>
+      <c r="K105" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>551</v>
       </c>
@@ -6519,8 +8048,17 @@
       <c r="H106" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I106">
+        <v>105</v>
+      </c>
+      <c r="J106" t="s">
+        <v>550</v>
+      </c>
+      <c r="K106" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>552</v>
       </c>
@@ -6545,8 +8083,17 @@
       <c r="H107" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I107">
+        <v>106</v>
+      </c>
+      <c r="J107" t="s">
+        <v>551</v>
+      </c>
+      <c r="K107" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>553</v>
       </c>
@@ -6571,8 +8118,17 @@
       <c r="H108" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I108">
+        <v>107</v>
+      </c>
+      <c r="J108" t="s">
+        <v>552</v>
+      </c>
+      <c r="K108" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>554</v>
       </c>
@@ -6597,8 +8153,17 @@
       <c r="H109" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I109">
+        <v>108</v>
+      </c>
+      <c r="J109" t="s">
+        <v>553</v>
+      </c>
+      <c r="K109" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>555</v>
       </c>
@@ -6623,8 +8188,17 @@
       <c r="H110" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I110">
+        <v>109</v>
+      </c>
+      <c r="J110" t="s">
+        <v>554</v>
+      </c>
+      <c r="K110" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>556</v>
       </c>
@@ -6649,8 +8223,17 @@
       <c r="H111" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I111">
+        <v>110</v>
+      </c>
+      <c r="J111" t="s">
+        <v>555</v>
+      </c>
+      <c r="K111" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>557</v>
       </c>
@@ -6672,8 +8255,17 @@
       <c r="H112" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I112">
+        <v>111</v>
+      </c>
+      <c r="J112" t="s">
+        <v>556</v>
+      </c>
+      <c r="K112" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B113">
         <v>2</v>
       </c>
@@ -6686,8 +8278,11 @@
       <c r="F113" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I113">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>562</v>
       </c>
@@ -6712,8 +8307,17 @@
       <c r="H114" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I114">
+        <v>113</v>
+      </c>
+      <c r="J114" t="s">
+        <v>557</v>
+      </c>
+      <c r="K114" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>563</v>
       </c>
@@ -6738,8 +8342,17 @@
       <c r="H115" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I115">
+        <v>114</v>
+      </c>
+      <c r="J115" t="s">
+        <v>562</v>
+      </c>
+      <c r="K115" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>564</v>
       </c>
@@ -6764,8 +8377,17 @@
       <c r="H116" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I116">
+        <v>115</v>
+      </c>
+      <c r="J116" t="s">
+        <v>563</v>
+      </c>
+      <c r="K116" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>565</v>
       </c>
@@ -6790,8 +8412,17 @@
       <c r="H117" s="4" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I117">
+        <v>116</v>
+      </c>
+      <c r="J117" t="s">
+        <v>564</v>
+      </c>
+      <c r="K117" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B118">
         <v>1</v>
       </c>
@@ -6801,8 +8432,11 @@
       <c r="F118" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I118">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B119">
         <v>2</v>
       </c>
@@ -6815,8 +8449,11 @@
       <c r="F119" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I119">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>558</v>
       </c>
@@ -6838,8 +8475,17 @@
       <c r="G120" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I120">
+        <v>119</v>
+      </c>
+      <c r="J120" t="s">
+        <v>565</v>
+      </c>
+      <c r="K120" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>559</v>
       </c>
@@ -6864,8 +8510,17 @@
       <c r="H121" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I121">
+        <v>120</v>
+      </c>
+      <c r="J121" t="s">
+        <v>558</v>
+      </c>
+      <c r="K121" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>560</v>
       </c>
@@ -6890,8 +8545,17 @@
       <c r="H122" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I122">
+        <v>121</v>
+      </c>
+      <c r="J122" t="s">
+        <v>559</v>
+      </c>
+      <c r="K122" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>561</v>
       </c>
@@ -6916,8 +8580,17 @@
       <c r="H123" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I123">
+        <v>122</v>
+      </c>
+      <c r="J123" t="s">
+        <v>560</v>
+      </c>
+      <c r="K123" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>566</v>
       </c>
@@ -6939,8 +8612,17 @@
       <c r="H124" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I124">
+        <v>123</v>
+      </c>
+      <c r="J124" t="s">
+        <v>561</v>
+      </c>
+      <c r="K124" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>567</v>
       </c>
@@ -6962,8 +8644,17 @@
       <c r="H125" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I125">
+        <v>124</v>
+      </c>
+      <c r="J125" t="s">
+        <v>566</v>
+      </c>
+      <c r="K125" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>568</v>
       </c>
@@ -6985,8 +8676,17 @@
       <c r="H126" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I126">
+        <v>125</v>
+      </c>
+      <c r="J126" t="s">
+        <v>567</v>
+      </c>
+      <c r="K126" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>569</v>
       </c>
@@ -7008,8 +8708,17 @@
       <c r="H127" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I127">
+        <v>126</v>
+      </c>
+      <c r="J127" t="s">
+        <v>568</v>
+      </c>
+      <c r="K127" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>570</v>
       </c>
@@ -7031,8 +8740,17 @@
       <c r="H128" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I128">
+        <v>127</v>
+      </c>
+      <c r="J128" t="s">
+        <v>569</v>
+      </c>
+      <c r="K128" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>571</v>
       </c>
@@ -7053,6 +8771,12 @@
       </c>
       <c r="H129" t="s">
         <v>463</v>
+      </c>
+      <c r="I129">
+        <v>128</v>
+      </c>
+      <c r="J129" t="s">
+        <v>570</v>
       </c>
     </row>
   </sheetData>

</xml_diff>